<commit_message>
Update USB protocol specification documents
 * Added protocol for notification of "device settings has changed by device itself" from device to host.
  - Name: ChangedSettingsByDevice
  - ReportId: 0x0A
  - MessageId: 0x02
 * NOTE: Basically, in EGS, host applications has device settings and set it to device when the application starts or a device is connected.
</commit_message>
<xml_diff>
--- a/Documents/UsbProtocol_EgsDeviceSettingsHidReport_CategoryList.xlsx
+++ b/Documents/UsbProtocol_EgsDeviceSettingsHidReport_CategoryList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kishimoto\Documents\exvision\PiemonteOnMyriad\HostApplications\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KISHIMOTO\Documents\Exvision\PiemonteOnMyriad\HostApplications\Windows\PublishedInGitHub\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="181">
   <si>
     <t>CategoryId</t>
   </si>
@@ -630,6 +630,30 @@
   <si>
     <t>UsbAndMiscs</t>
     <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ChangedSettingsByDevice</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>0x0D</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>EgsGestureOnMouseOrSingleTouchMode</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>0x1C</t>
+    <phoneticPr fontId="20"/>
+  </si>
+  <si>
+    <t>EgsDeviceFirmwareUpdate (Fast Transfer)</t>
+    <phoneticPr fontId="20"/>
   </si>
 </sst>
 </file>
@@ -1236,7 +1260,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1260,6 +1284,12 @@
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1588,16 +1618,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN47"/>
+  <dimension ref="A1:BN50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="10.625" style="1" customWidth="1"/>
@@ -1820,74 +1850,74 @@
       <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="8" t="s">
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8" t="s">
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8" t="s">
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="8"/>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="8"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="8"/>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="8"/>
-      <c r="AX2" s="8"/>
-      <c r="AY2" s="8"/>
-      <c r="AZ2" s="8"/>
-      <c r="BA2" s="8"/>
-      <c r="BB2" s="8"/>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="8"/>
-      <c r="BF2" s="8"/>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="8"/>
-      <c r="BI2" s="8"/>
-      <c r="BJ2" s="8"/>
-      <c r="BK2" s="8"/>
-      <c r="BL2" s="8"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="8"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="10"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="10"/>
+      <c r="BL2" s="10"/>
+      <c r="BM2" s="10"/>
+      <c r="BN2" s="10"/>
     </row>
     <row r="3" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B3" s="1" t="s">
@@ -1902,18 +1932,18 @@
       <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8" t="s">
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
     </row>
     <row r="4" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
@@ -2106,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>89</v>
       </c>
@@ -2120,7 +2150,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
         <v>174</v>
       </c>
@@ -2134,7 +2164,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
         <v>29</v>
       </c>
@@ -2148,7 +2178,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
         <v>160</v>
       </c>
@@ -2158,30 +2188,30 @@
       <c r="D20" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
         <v>166</v>
       </c>
@@ -2195,7 +2225,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
         <v>163</v>
       </c>
@@ -2205,30 +2235,30 @@
       <c r="D23" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+    </row>
+    <row r="24" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>68</v>
       </c>
@@ -2251,7 +2281,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:66" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B26" s="6" t="s">
         <v>171</v>
       </c>
@@ -2270,7 +2300,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
@@ -2286,12 +2316,12 @@
       <c r="F27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H27" s="9"/>
-    </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H27" s="11"/>
+    </row>
+    <row r="28" spans="1:66" s="4" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B28" s="4" t="s">
         <v>169</v>
       </c>
@@ -2310,12 +2340,12 @@
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:66" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>64</v>
       </c>
@@ -2326,111 +2356,188 @@
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="B32" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C32" s="1" t="s">
+    <row r="32" spans="1:66" s="8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>57</v>
-      </c>
+      <c r="D32" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+      <c r="W32" s="10"/>
+      <c r="X32" s="10"/>
+      <c r="Y32" s="10"/>
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="10"/>
+      <c r="AB32" s="10"/>
+      <c r="AC32" s="10"/>
+      <c r="AD32" s="10"/>
+      <c r="AE32" s="10"/>
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="10"/>
+      <c r="AH32" s="10"/>
+      <c r="AI32" s="10"/>
+      <c r="AJ32" s="10"/>
+      <c r="AK32" s="10"/>
+      <c r="AL32" s="10"/>
+      <c r="AM32" s="10"/>
+      <c r="AN32" s="10"/>
+      <c r="AO32" s="10"/>
+      <c r="AP32" s="10"/>
+      <c r="AQ32" s="10"/>
+      <c r="AR32" s="10"/>
+      <c r="AS32" s="10"/>
+      <c r="AT32" s="10"/>
+      <c r="AU32" s="10"/>
+      <c r="AV32" s="10"/>
+      <c r="AW32" s="10"/>
+      <c r="AX32" s="10"/>
+      <c r="AY32" s="10"/>
+      <c r="AZ32" s="10"/>
+      <c r="BA32" s="10"/>
+      <c r="BB32" s="10"/>
+      <c r="BC32" s="10"/>
+      <c r="BD32" s="10"/>
+      <c r="BE32" s="10"/>
+      <c r="BF32" s="10"/>
+      <c r="BG32" s="10"/>
+      <c r="BH32" s="10"/>
+      <c r="BI32" s="10"/>
+      <c r="BJ32" s="10"/>
+      <c r="BK32" s="10"/>
+      <c r="BL32" s="10"/>
+      <c r="BM32" s="10"/>
+      <c r="BN32" s="10"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B37" s="1" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B38" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B38" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B39" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B40" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B41" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B42" s="2" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B43" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B44" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B45" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>44</v>
@@ -2438,22 +2545,50 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B47" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B49" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B47" s="2" t="s">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B50" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="13">
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="O32:R32"/>
+    <mergeCell ref="S32:BN32"/>
     <mergeCell ref="S2:BN2"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G2:J2"/>

</xml_diff>